<commit_message>
add auto change mde
</commit_message>
<xml_diff>
--- a/raports/raport-05-27-21_11;45.xlsx
+++ b/raports/raport-05-27-21_11;45.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -624,21 +624,21 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>35325</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>617722</v>
+        <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19256.9/s </t>
+          <t xml:space="preserve"> 9294.6/s </t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>7028.786035987406</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>19.96071533796785</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -647,7 +647,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>100%Success</t>
+          <t>75%Success</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -666,21 +666,21 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>31290</v>
+        <v>17625</v>
       </c>
       <c r="C7" t="n">
-        <v>497761</v>
+        <v>219236</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15282.8/s </t>
+          <t xml:space="preserve"> 4733.5/s </t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5574.277247209994</v>
+        <v>1530.547913558057</v>
       </c>
       <c r="F7" t="n">
-        <v>28.08259184628731</v>
+        <v>60.89500811910357</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -689,7 +689,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>95%Success</t>
+          <t>70%Success</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -699,7 +699,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -708,21 +708,21 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>18465</v>
+        <v>7860</v>
       </c>
       <c r="C8" t="n">
-        <v>436569</v>
+        <v>437392</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 13070.1/s </t>
+          <t xml:space="preserve"> 13840.2/s </t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>4766.905023924121</v>
+        <v>5048.718359723461</v>
       </c>
       <c r="F8" t="n">
-        <v>32.90381131046819</v>
+        <v>19.02445403665375</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>90%Success</t>
+          <t>100%Success</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -750,21 +750,21 @@
         <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>21720</v>
+        <v>8415</v>
       </c>
       <c r="C9" t="n">
-        <v>394642</v>
+        <v>509238</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 8461.6/s </t>
+          <t xml:space="preserve"> 15535.0/s </t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3084.919072799978</v>
+        <v>5661.700839115933</v>
       </c>
       <c r="F9" t="n">
-        <v>36.92881903091973</v>
+        <v>25.66828477057825</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -773,7 +773,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>85%Success</t>
+          <t>95%Success</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -792,21 +792,21 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>15810</v>
+        <v>25170</v>
       </c>
       <c r="C10" t="n">
-        <v>356948</v>
+        <v>431379</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5770.4/s </t>
+          <t xml:space="preserve"> 12395.2/s </t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2101.542480619212</v>
+        <v>4526.671226067946</v>
       </c>
       <c r="F10" t="n">
-        <v>42.19766184430253</v>
+        <v>31.13852551932311</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>80%Success</t>
+          <t>90%Success</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -834,21 +834,21 @@
         <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>18090</v>
+        <v>17610</v>
       </c>
       <c r="C11" t="n">
-        <v>326489</v>
+        <v>396499</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5270.5/s </t>
+          <t xml:space="preserve"> 6599.1/s </t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1921.601808769367</v>
+        <v>2404.019495873922</v>
       </c>
       <c r="F11" t="n">
-        <v>46.64337542765448</v>
+        <v>34.71681139170617</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>75%Success</t>
+          <t>85%Success</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -876,21 +876,21 @@
         <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>20145</v>
+        <v>16695</v>
       </c>
       <c r="C12" t="n">
-        <v>227577</v>
+        <v>356787</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5019.5/s </t>
+          <t xml:space="preserve"> 4138.2/s </t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1831.448605061528</v>
+        <v>1506.000210839302</v>
       </c>
       <c r="F12" t="n">
-        <v>66.30804958321683</v>
+        <v>40.23573728863409</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -899,7 +899,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>70%Success</t>
+          <t>80%Success</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -918,38 +918,416 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
+        <v>14235</v>
+      </c>
+      <c r="C13" t="n">
+        <v>325359</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5193.6/s </t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1892.590185189449</v>
+      </c>
+      <c r="F13" t="n">
+        <v>45.08529962287786</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>75%Success</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>14550</v>
+      </c>
+      <c r="C14" t="n">
+        <v>295284</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3141.5/s </t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1144.051285127713</v>
+      </c>
+      <c r="F14" t="n">
+        <v>50.49084271413308</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>70%Success</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>35325</v>
+      </c>
+      <c r="C15" t="n">
+        <v>617722</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 19256.9/s </t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>7028.786035987406</v>
+      </c>
+      <c r="F15" t="n">
+        <v>19.96071533796785</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>100%Success</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>31290</v>
+      </c>
+      <c r="C16" t="n">
+        <v>497761</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15282.8/s </t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>5574.277247209994</v>
+      </c>
+      <c r="F16" t="n">
+        <v>28.08259184628731</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>95%Success</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>18465</v>
+      </c>
+      <c r="C17" t="n">
+        <v>436569</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13070.1/s </t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>4766.905023924121</v>
+      </c>
+      <c r="F17" t="n">
+        <v>32.90381131046819</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>90%Success</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>21720</v>
+      </c>
+      <c r="C18" t="n">
+        <v>394642</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8461.6/s </t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>3084.919072799978</v>
+      </c>
+      <c r="F18" t="n">
+        <v>36.92881903091973</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>85%Success</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>15810</v>
+      </c>
+      <c r="C19" t="n">
+        <v>356948</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5770.4/s </t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>2101.542480619212</v>
+      </c>
+      <c r="F19" t="n">
+        <v>42.19766184430253</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>80%Success</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>18090</v>
+      </c>
+      <c r="C20" t="n">
+        <v>326489</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5270.5/s </t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>1921.601808769367</v>
+      </c>
+      <c r="F20" t="n">
+        <v>46.64337542765448</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>75%Success</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20145</v>
+      </c>
+      <c r="C21" t="n">
+        <v>227577</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5019.5/s </t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>1831.448605061528</v>
+      </c>
+      <c r="F21" t="n">
+        <v>66.30804958321683</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>70%Success</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0</v>
+      </c>
+      <c r="B22" t="n">
         <v>29160</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C22" t="n">
         <v>397993</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t xml:space="preserve"> 12562.9/s </t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="E22" t="n">
         <v>4579.936777162606</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F22" t="n">
         <v>37.13373602048266</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>short</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>100%Success</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>apm</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>apm</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>